<commit_message>
read only defined columns
</commit_message>
<xml_diff>
--- a/testdata/test1.xlsx
+++ b/testdata/test1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Text</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve">something</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The same</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a table</t>
   </si>
 </sst>
 </file>
@@ -392,14 +398,14 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,8 +444,21 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>42</v>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4534567</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f aca="false">IF(AND($A3&lt;&gt;"",$B3&lt;&gt;"",$D3&lt;&gt;""),"Filled","Not filled")</f>
+        <v>Filled</v>
       </c>
     </row>
   </sheetData>

</xml_diff>